<commit_message>
just did some test calculations in these files--nothing was actually changed
</commit_message>
<xml_diff>
--- a/RawData/cropfertrates.xlsx
+++ b/RawData/cropfertrates.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/malgren/Documents/Mines/N_P/NANI_NAPI/NANI_NAPI_R/RawData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/malgren/Documents/Mines/N_P/NANI_NAPI/CSNAPNIv1/RawData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65820A5A-856A-DE44-8D3F-16307E024BDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BCD7722-60F4-7643-9FC0-E3E34FB96151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="-21380" windowWidth="21780" windowHeight="17440" activeTab="3" xr2:uid="{ACD52FB1-2477-7646-B2ED-4056C048DD2A}"/>
+    <workbookView xWindow="7420" yWindow="680" windowWidth="28760" windowHeight="19660" activeTab="4" xr2:uid="{ACD52FB1-2477-7646-B2ED-4056C048DD2A}"/>
   </bookViews>
   <sheets>
     <sheet name="Nfert" sheetId="3" r:id="rId1"/>
     <sheet name="Pfert" sheetId="2" r:id="rId2"/>
     <sheet name="Nfert_old" sheetId="1" r:id="rId3"/>
     <sheet name="Pfert_P2O5" sheetId="4" r:id="rId4"/>
+    <sheet name="N_P_ratio" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="38">
   <si>
     <t>N inputs to crops in lbs/acre</t>
   </si>
@@ -148,11 +149,17 @@
   <si>
     <t>P inputs to crops in metric tons/km2</t>
   </si>
+  <si>
+    <t>N/P inputs to crops in lbs/acre</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="0.0"/>
+  </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -275,7 +282,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -311,6 +318,11 @@
     <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -628,7 +640,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50B754A4-6FA9-FA43-A8B4-C06FEAEE0E02}">
   <dimension ref="A1:O42"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D41" sqref="D41:D42"/>
     </sheetView>
   </sheetViews>
@@ -1941,7 +1953,7 @@
   <dimension ref="A1:K42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+      <selection sqref="A1:H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3834,7 +3846,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6C257C3-61A3-694F-B375-9FAAD761AFA8}">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
@@ -4341,4 +4353,658 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057CC99-4510-2A4A-94DF-11409CC16956}">
+  <dimension ref="A1:P18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1:P18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="14" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="25"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2">
+        <v>1987</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1992</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1997</v>
+      </c>
+      <c r="E2" s="2">
+        <v>2002</v>
+      </c>
+      <c r="F2" s="2">
+        <v>2007</v>
+      </c>
+      <c r="G2" s="2">
+        <v>2012</v>
+      </c>
+      <c r="H2" s="2">
+        <v>2017</v>
+      </c>
+      <c r="M2" s="26"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="26"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="17">
+        <f>Nfert!B3/Pfert!B3</f>
+        <v>5.7356759272941371</v>
+      </c>
+      <c r="C3" s="17">
+        <f>Nfert!C3/Pfert!C3</f>
+        <v>6.0399607371220299</v>
+      </c>
+      <c r="D3" s="17">
+        <f>Nfert!D3/Pfert!D3</f>
+        <v>6.1598732158941107</v>
+      </c>
+      <c r="E3" s="17">
+        <f>Nfert!E3/Pfert!E3</f>
+        <v>6.358590060613988</v>
+      </c>
+      <c r="F3" s="17">
+        <f>Nfert!F3/Pfert!F3</f>
+        <v>6.5336265706689396</v>
+      </c>
+      <c r="G3" s="17">
+        <f>Nfert!G3/Pfert!G3</f>
+        <v>6.2791076848563128</v>
+      </c>
+      <c r="H3" s="17">
+        <f>Nfert!H3/Pfert!H3</f>
+        <v>6.3967469563314578</v>
+      </c>
+      <c r="M3" s="27"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="28"/>
+      <c r="P3" s="29"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="17">
+        <f>Nfert!B4/Pfert!B4</f>
+        <v>5.7356759272941371</v>
+      </c>
+      <c r="C4" s="17">
+        <f>Nfert!C4/Pfert!C4</f>
+        <v>6.0399607371220299</v>
+      </c>
+      <c r="D4" s="17">
+        <f>Nfert!D4/Pfert!D4</f>
+        <v>6.1598732158941107</v>
+      </c>
+      <c r="E4" s="17">
+        <f>Nfert!E4/Pfert!E4</f>
+        <v>6.358590060613988</v>
+      </c>
+      <c r="F4" s="17">
+        <f>Nfert!F4/Pfert!F4</f>
+        <v>6.5336265706689396</v>
+      </c>
+      <c r="G4" s="17">
+        <f>Nfert!G4/Pfert!G4</f>
+        <v>6.2791076848563128</v>
+      </c>
+      <c r="H4" s="17">
+        <f>Nfert!H4/Pfert!H4</f>
+        <v>6.3967469563314578</v>
+      </c>
+      <c r="M4" s="27"/>
+      <c r="N4" s="28"/>
+      <c r="O4" s="28"/>
+      <c r="P4" s="29"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="17">
+        <f>Nfert!B5/Pfert!B5</f>
+        <v>6.4951770838138296</v>
+      </c>
+      <c r="C5" s="17">
+        <f>Nfert!C5/Pfert!C5</f>
+        <v>6.2935989703033304</v>
+      </c>
+      <c r="D5" s="17">
+        <f>Nfert!D5/Pfert!D5</f>
+        <v>6.5288365218634627</v>
+      </c>
+      <c r="E5" s="17">
+        <f>Nfert!E5/Pfert!E5</f>
+        <v>6.381686086381599</v>
+      </c>
+      <c r="F5" s="17">
+        <f>Nfert!F5/Pfert!F5</f>
+        <v>6.0019277488199032</v>
+      </c>
+      <c r="G5" s="17">
+        <f>Nfert!G5/Pfert!G5</f>
+        <v>6.4962041516638953</v>
+      </c>
+      <c r="H5" s="17">
+        <f>Nfert!H5/Pfert!H5</f>
+        <v>11.862633668255809</v>
+      </c>
+      <c r="M5" s="27"/>
+      <c r="N5" s="28"/>
+      <c r="O5" s="28"/>
+      <c r="P5" s="29"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="17">
+        <f>Nfert!B6/Pfert!B6</f>
+        <v>4.9443864417519636</v>
+      </c>
+      <c r="C6" s="17">
+        <f>Nfert!C6/Pfert!C6</f>
+        <v>4.9443864417519636</v>
+      </c>
+      <c r="D6" s="17">
+        <f>Nfert!D6/Pfert!D6</f>
+        <v>4.9443864417519636</v>
+      </c>
+      <c r="E6" s="17">
+        <f>Nfert!E6/Pfert!E6</f>
+        <v>4.9443864417519636</v>
+      </c>
+      <c r="F6" s="17">
+        <f>Nfert!F6/Pfert!F6</f>
+        <v>4.9443864417519636</v>
+      </c>
+      <c r="G6" s="17">
+        <f>Nfert!G6/Pfert!G6</f>
+        <v>4.9443864417519636</v>
+      </c>
+      <c r="H6" s="17">
+        <f>Nfert!H6/Pfert!H6</f>
+        <v>4.9443864417519645</v>
+      </c>
+      <c r="M6" s="27"/>
+      <c r="N6" s="28"/>
+      <c r="O6" s="28"/>
+      <c r="P6" s="29"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="17">
+        <f>Nfert!B7/Pfert!B7</f>
+        <v>7.0468274251375851</v>
+      </c>
+      <c r="C7" s="17">
+        <f>Nfert!C7/Pfert!C7</f>
+        <v>7.0468274251375851</v>
+      </c>
+      <c r="D7" s="17">
+        <f>Nfert!D7/Pfert!D7</f>
+        <v>7.0468274251375851</v>
+      </c>
+      <c r="E7" s="17">
+        <f>Nfert!E7/Pfert!E7</f>
+        <v>7.0468274251375851</v>
+      </c>
+      <c r="F7" s="17">
+        <f>Nfert!F7/Pfert!F7</f>
+        <v>7.0468274251375851</v>
+      </c>
+      <c r="G7" s="17">
+        <f>Nfert!G7/Pfert!G7</f>
+        <v>7.0468274251375851</v>
+      </c>
+      <c r="H7" s="17">
+        <f>Nfert!H7/Pfert!H7</f>
+        <v>7.0468274251375842</v>
+      </c>
+      <c r="M7" s="27"/>
+      <c r="N7" s="28"/>
+      <c r="O7" s="28"/>
+      <c r="P7" s="29"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="17">
+        <f>Nfert!B8/Pfert!B8</f>
+        <v>9.7288140812736739</v>
+      </c>
+      <c r="C8" s="17">
+        <f>Nfert!C8/Pfert!C8</f>
+        <v>9.7288140812736739</v>
+      </c>
+      <c r="D8" s="17">
+        <f>Nfert!D8/Pfert!D8</f>
+        <v>9.7288140812736739</v>
+      </c>
+      <c r="E8" s="17">
+        <f>Nfert!E8/Pfert!E8</f>
+        <v>9.7288140812736739</v>
+      </c>
+      <c r="F8" s="17">
+        <f>Nfert!F8/Pfert!F8</f>
+        <v>9.2729018141949116</v>
+      </c>
+      <c r="G8" s="17">
+        <f>Nfert!G8/Pfert!G8</f>
+        <v>8.7821224136618863</v>
+      </c>
+      <c r="H8" s="17">
+        <f>Nfert!H8/Pfert!H8</f>
+        <v>8.7821224136618845</v>
+      </c>
+      <c r="M8" s="27"/>
+      <c r="N8" s="28"/>
+      <c r="O8" s="28"/>
+      <c r="P8" s="29"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="17">
+        <f>Nfert!B9/Pfert!B9</f>
+        <v>9.7288140812736739</v>
+      </c>
+      <c r="C9" s="17">
+        <f>Nfert!C9/Pfert!C9</f>
+        <v>9.7288140812736739</v>
+      </c>
+      <c r="D9" s="17">
+        <f>Nfert!D9/Pfert!D9</f>
+        <v>9.7288140812736739</v>
+      </c>
+      <c r="E9" s="17">
+        <f>Nfert!E9/Pfert!E9</f>
+        <v>9.7288140812736739</v>
+      </c>
+      <c r="F9" s="17">
+        <f>Nfert!F9/Pfert!F9</f>
+        <v>9.2729018141949116</v>
+      </c>
+      <c r="G9" s="17">
+        <f>Nfert!G9/Pfert!G9</f>
+        <v>8.7821224136618863</v>
+      </c>
+      <c r="H9" s="17">
+        <f>Nfert!H9/Pfert!H9</f>
+        <v>8.7821224136618845</v>
+      </c>
+      <c r="M9" s="27"/>
+      <c r="N9" s="28"/>
+      <c r="O9" s="28"/>
+      <c r="P9" s="29"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="17">
+        <f>Nfert!B10/Pfert!B10</f>
+        <v>2.8302748946531451</v>
+      </c>
+      <c r="C10" s="17">
+        <f>Nfert!C10/Pfert!C10</f>
+        <v>2.9116893976983778</v>
+      </c>
+      <c r="D10" s="17">
+        <f>Nfert!D10/Pfert!D10</f>
+        <v>3.0789109880309895</v>
+      </c>
+      <c r="E10" s="17">
+        <f>Nfert!E10/Pfert!E10</f>
+        <v>3.1766841083080548</v>
+      </c>
+      <c r="F10" s="17">
+        <f>Nfert!F10/Pfert!F10</f>
+        <v>3.2580614926442166</v>
+      </c>
+      <c r="G10" s="17">
+        <f>Nfert!G10/Pfert!G10</f>
+        <v>3.5488585035235318</v>
+      </c>
+      <c r="H10" s="17">
+        <f>Nfert!H10/Pfert!H10</f>
+        <v>3.3603510079553072</v>
+      </c>
+      <c r="M10" s="27"/>
+      <c r="N10" s="28"/>
+      <c r="O10" s="28"/>
+      <c r="P10" s="29"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="17">
+        <f>Nfert!B11/Pfert!B11</f>
+        <v>4.5870290999636749</v>
+      </c>
+      <c r="C11" s="17">
+        <f>Nfert!C11/Pfert!C11</f>
+        <v>4.5870290999636749</v>
+      </c>
+      <c r="D11" s="17">
+        <f>Nfert!D11/Pfert!D11</f>
+        <v>4.5870290999636749</v>
+      </c>
+      <c r="E11" s="17">
+        <f>Nfert!E11/Pfert!E11</f>
+        <v>4.5870290999636749</v>
+      </c>
+      <c r="F11" s="17">
+        <f>Nfert!F11/Pfert!F11</f>
+        <v>4.5870290999636749</v>
+      </c>
+      <c r="G11" s="17">
+        <f>Nfert!G11/Pfert!G11</f>
+        <v>4.5870290999636749</v>
+      </c>
+      <c r="H11" s="17">
+        <f>Nfert!H11/Pfert!H11</f>
+        <v>4.5870290999636749</v>
+      </c>
+      <c r="M11" s="27"/>
+      <c r="N11" s="28"/>
+      <c r="O11" s="28"/>
+      <c r="P11" s="29"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="17">
+        <f>Nfert!B12/Pfert!B12</f>
+        <v>1.5286693906845339</v>
+      </c>
+      <c r="C12" s="17">
+        <f>Nfert!C12/Pfert!C12</f>
+        <v>1.5286693906845339</v>
+      </c>
+      <c r="D12" s="17">
+        <f>Nfert!D12/Pfert!D12</f>
+        <v>1.5286693906845339</v>
+      </c>
+      <c r="E12" s="17">
+        <f>Nfert!E12/Pfert!E12</f>
+        <v>1.5286693906845339</v>
+      </c>
+      <c r="F12" s="17">
+        <f>Nfert!F12/Pfert!F12</f>
+        <v>1.5286693906845339</v>
+      </c>
+      <c r="G12" s="17">
+        <f>Nfert!G12/Pfert!G12</f>
+        <v>1.5286693906845339</v>
+      </c>
+      <c r="H12" s="17">
+        <f>Nfert!H12/Pfert!H12</f>
+        <v>1.5286693906845339</v>
+      </c>
+      <c r="M12" s="27"/>
+      <c r="N12" s="28"/>
+      <c r="O12" s="28"/>
+      <c r="P12" s="29"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="17">
+        <f>Nfert!B13/Pfert!B13</f>
+        <v>1.5286693906845339</v>
+      </c>
+      <c r="C13" s="17">
+        <f>Nfert!C13/Pfert!C13</f>
+        <v>1.5286693906845339</v>
+      </c>
+      <c r="D13" s="17">
+        <f>Nfert!D13/Pfert!D13</f>
+        <v>1.5286693906845339</v>
+      </c>
+      <c r="E13" s="17">
+        <f>Nfert!E13/Pfert!E13</f>
+        <v>1.5286693906845339</v>
+      </c>
+      <c r="F13" s="17">
+        <f>Nfert!F13/Pfert!F13</f>
+        <v>1.5286693906845339</v>
+      </c>
+      <c r="G13" s="17">
+        <f>Nfert!G13/Pfert!G13</f>
+        <v>1.5286693906845339</v>
+      </c>
+      <c r="H13" s="17">
+        <f>Nfert!H13/Pfert!H13</f>
+        <v>1.5286693906845339</v>
+      </c>
+      <c r="M13" s="27"/>
+      <c r="N13" s="28"/>
+      <c r="O13" s="28"/>
+      <c r="P13" s="29"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="17">
+        <f>Nfert!B14/Pfert!B14</f>
+        <v>0.58510088692557671</v>
+      </c>
+      <c r="C14" s="17">
+        <f>Nfert!C14/Pfert!C14</f>
+        <v>0.73137610865697078</v>
+      </c>
+      <c r="D14" s="17">
+        <f>Nfert!D14/Pfert!D14</f>
+        <v>0.81844469302089595</v>
+      </c>
+      <c r="E14" s="17">
+        <f>Nfert!E14/Pfert!E14</f>
+        <v>0.75548740894236555</v>
+      </c>
+      <c r="F14" s="17">
+        <f>Nfert!F14/Pfert!F14</f>
+        <v>0.56617115234857274</v>
+      </c>
+      <c r="G14" s="17">
+        <f>Nfert!G14/Pfert!G14</f>
+        <v>0.54605113109656689</v>
+      </c>
+      <c r="H14" s="17">
+        <f>Nfert!H14/Pfert!H14</f>
+        <v>0.59978329661156082</v>
+      </c>
+      <c r="M14" s="27"/>
+      <c r="N14" s="28"/>
+      <c r="O14" s="28"/>
+      <c r="P14" s="29"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="17" t="e">
+        <f>Nfert!B15/Pfert!B15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C15" s="17" t="e">
+        <f>Nfert!C15/Pfert!C15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D15" s="17" t="e">
+        <f>Nfert!D15/Pfert!D15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E15" s="17" t="e">
+        <f>Nfert!E15/Pfert!E15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F15" s="17" t="e">
+        <f>Nfert!F15/Pfert!F15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G15" s="17" t="e">
+        <f>Nfert!G15/Pfert!G15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H15" s="17" t="e">
+        <f>Nfert!H15/Pfert!H15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M15" s="27"/>
+      <c r="N15" s="28"/>
+      <c r="O15" s="28"/>
+      <c r="P15" s="29"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="17" t="e">
+        <f>Nfert!B16/Pfert!B16</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C16" s="17" t="e">
+        <f>Nfert!C16/Pfert!C16</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D16" s="17" t="e">
+        <f>Nfert!D16/Pfert!D16</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E16" s="17" t="e">
+        <f>Nfert!E16/Pfert!E16</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F16" s="17" t="e">
+        <f>Nfert!F16/Pfert!F16</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G16" s="17" t="e">
+        <f>Nfert!G16/Pfert!G16</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H16" s="17" t="e">
+        <f>Nfert!H16/Pfert!H16</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M16" s="27"/>
+      <c r="N16" s="28"/>
+      <c r="O16" s="28"/>
+      <c r="P16" s="29"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="17">
+        <f>Nfert!B17/Pfert!B17</f>
+        <v>11.512584064943493</v>
+      </c>
+      <c r="C17" s="17">
+        <f>Nfert!C17/Pfert!C17</f>
+        <v>11.512584064943493</v>
+      </c>
+      <c r="D17" s="17">
+        <f>Nfert!D17/Pfert!D17</f>
+        <v>11.512584064943493</v>
+      </c>
+      <c r="E17" s="17">
+        <f>Nfert!E17/Pfert!E17</f>
+        <v>11.512584064943493</v>
+      </c>
+      <c r="F17" s="17">
+        <f>Nfert!F17/Pfert!F17</f>
+        <v>11.512584064943493</v>
+      </c>
+      <c r="G17" s="17">
+        <f>Nfert!G17/Pfert!G17</f>
+        <v>9.6355543760600764</v>
+      </c>
+      <c r="H17" s="17">
+        <f>Nfert!H17/Pfert!H17</f>
+        <v>9.6355543760600764</v>
+      </c>
+      <c r="M17" s="27"/>
+      <c r="N17" s="28"/>
+      <c r="O17" s="28"/>
+      <c r="P17" s="29"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="17">
+        <f>Nfert!B18/Pfert!B18</f>
+        <v>1.8132741647884192</v>
+      </c>
+      <c r="C18" s="17">
+        <f>Nfert!C18/Pfert!C18</f>
+        <v>1.8132741647884192</v>
+      </c>
+      <c r="D18" s="17">
+        <f>Nfert!D18/Pfert!D18</f>
+        <v>1.8132741647884192</v>
+      </c>
+      <c r="E18" s="17">
+        <f>Nfert!E18/Pfert!E18</f>
+        <v>1.4453025958926806</v>
+      </c>
+      <c r="F18" s="17">
+        <f>Nfert!F18/Pfert!F18</f>
+        <v>1.4453025958926806</v>
+      </c>
+      <c r="G18" s="17">
+        <f>Nfert!G18/Pfert!G18</f>
+        <v>1.5670798495298948</v>
+      </c>
+      <c r="H18" s="17">
+        <f>Nfert!H18/Pfert!H18</f>
+        <v>1.5670798495298948</v>
+      </c>
+      <c r="M18" s="27"/>
+      <c r="N18" s="29"/>
+      <c r="O18" s="29"/>
+      <c r="P18" s="29"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>